<commit_message>
Updates at the end of Sprint 3
</commit_message>
<xml_diff>
--- a/Deliverables/Agile/Sprint Metrics.xlsx
+++ b/Deliverables/Agile/Sprint Metrics.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Metric</t>
   </si>
@@ -504,7 +504,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,7 +512,7 @@
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -559,7 +559,9 @@
       <c r="C3" s="4">
         <v>2</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4">
+        <v>3</v>
+      </c>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" ht="42" x14ac:dyDescent="0.35">
@@ -587,7 +589,9 @@
       <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" s="8" customFormat="1" ht="76.5" x14ac:dyDescent="0.35">
@@ -605,7 +609,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" ht="61.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="8" customFormat="1" ht="76.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -615,7 +619,9 @@
       <c r="C7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="E7" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates at start of Sprint 4
</commit_message>
<xml_diff>
--- a/Deliverables/Agile/Sprint Metrics.xlsx
+++ b/Deliverables/Agile/Sprint Metrics.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Metric</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>1.  Government manage all opportunities</t>
+  </si>
+  <si>
+    <t>1.  Government publish opportunity.  2.  Contractor view published opportunities</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D7"/>
+      <selection activeCell="F6" sqref="F6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +516,7 @@
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -546,7 +549,9 @@
       <c r="D2" s="4">
         <v>3</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="42" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
@@ -577,7 +582,9 @@
       <c r="D4" s="5">
         <v>1</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="42" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
@@ -594,7 +601,7 @@
       </c>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" ht="76.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="8" customFormat="1" ht="151.5" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
@@ -607,7 +614,9 @@
       <c r="D6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:5" s="8" customFormat="1" ht="76.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">

</xml_diff>

<commit_message>
Updates from Sprint 4 (FINAL)
</commit_message>
<xml_diff>
--- a/Deliverables/Agile/Sprint Metrics.xlsx
+++ b/Deliverables/Agile/Sprint Metrics.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Metric</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>1.  Government publish opportunity.  2.  Contractor view published opportunities</t>
+  </si>
+  <si>
+    <t>1.  Government publish opportunity.  2.  Contractor view published opportunities              3.  Government edit opportunity</t>
   </si>
 </sst>
 </file>
@@ -506,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:G6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +570,9 @@
       <c r="D3" s="4">
         <v>3</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="42" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
@@ -599,7 +604,9 @@
       <c r="D5" s="5">
         <v>1</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:5" s="8" customFormat="1" ht="151.5" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
@@ -618,7 +625,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" ht="76.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="8" customFormat="1" ht="121.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -631,7 +638,9 @@
       <c r="D7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>